<commit_message>
Update resume and salaries
</commit_message>
<xml_diff>
--- a/salary-transparency.xlsx
+++ b/salary-transparency.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcali\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcali\Desktop\Repositories\pingzing.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23BC1865-F89C-4C2B-B77D-5607ED496F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC6F034-8E78-41F2-B58F-C7A76FBE0DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3DD130F-2BA7-4CF7-A266-8FC2D1A3BE0F}"/>
   </bookViews>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
   <si>
     <t>Title</t>
   </si>
@@ -170,12 +162,6 @@
     <t>2021-05-17</t>
   </si>
   <si>
-    <t>Current</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>€5500 EUR / month</t>
   </si>
   <si>
@@ -204,6 +190,24 @@
   </si>
   <si>
     <t>EUR</t>
+  </si>
+  <si>
+    <t>2023-07-30</t>
+  </si>
+  <si>
+    <t>Senior Developer</t>
+  </si>
+  <si>
+    <t>2023-08-01</t>
+  </si>
+  <si>
+    <t>2023-08-31</t>
+  </si>
+  <si>
+    <t>€7500 EUR / month</t>
+  </si>
+  <si>
+    <t>Terminated</t>
   </si>
 </sst>
 </file>
@@ -429,19 +433,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$C$13</c15:sqref>
-                  </c15:fullRef>
-                  <c15:levelRef>
-                    <c15:sqref>Sheet1!$B$2:$B$13</c15:sqref>
-                  </c15:levelRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
+              <c:f>Sheet1!$B$2:$B$14</c:f>
               <c:strCache>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>2013-06-01</c:v>
                 </c:pt>
@@ -477,16 +471,19 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2022-05-01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2023-08-01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$13</c:f>
+              <c:f>Sheet1!$G$2:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
                 </c:pt>
@@ -522,6 +519,9 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>70200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>90000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -569,65 +569,101 @@
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>Sheet1!$B$2:$C$13</c15:sqref>
-                  </c15:fullRef>
-                  <c15:levelRef>
-                    <c15:sqref>Sheet1!$B$2:$B$13</c15:sqref>
-                  </c15:levelRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>Sheet1!$B$2:$B$13</c:f>
-              <c:strCache>
-                <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>2013-06-01</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2014-06-01</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2015-04-13</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2016-09-01</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2017-01-01</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2017-07-01</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2018-02-01</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2019-04-01</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2020-01-27</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2020-08-01</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2021-05-17</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2022-05-01</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$B$2:$C$14</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="13"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2014-06-01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2015-03-26</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2016-08-31</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2016-12-31</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2017-06-30</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2018-01-31</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2019-03-31</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2020-01-17</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2020-07-31</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2021-04-30</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2022-04-30</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2023-07-30</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2023-08-31</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2013-06-01</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2014-06-01</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2015-04-13</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2016-09-01</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2017-01-01</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2017-07-01</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>2018-02-01</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2019-04-01</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2020-01-27</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2020-08-01</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2021-05-17</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2022-05-01</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>2023-08-01</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$D$2:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>365</c:v>
                 </c:pt>
@@ -660,6 +696,12 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>364</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -764,7 +806,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2940000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1644,15 +1686,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>47624</xdr:rowOff>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1581149</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1977,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDAF2D-9C38-457B-A68E-C11A0F37BCCC}">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2014,10 +2056,10 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -2043,7 +2085,7 @@
         <v>48000</v>
       </c>
       <c r="H2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -2069,7 +2111,7 @@
         <v>57600</v>
       </c>
       <c r="H3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2089,13 +2131,13 @@
         <v>23</v>
       </c>
       <c r="F4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G4" s="5">
         <v>30252</v>
       </c>
       <c r="H4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2115,13 +2157,13 @@
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G5" s="5">
         <v>32767</v>
       </c>
       <c r="H5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2141,13 +2183,13 @@
         <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G6" s="5">
         <v>38640</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2167,13 +2209,13 @@
         <v>26</v>
       </c>
       <c r="F7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G7" s="5">
         <v>42684</v>
       </c>
       <c r="H7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2193,13 +2235,13 @@
         <v>31</v>
       </c>
       <c r="F8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G8" s="5">
         <v>47312</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2225,7 +2267,7 @@
         <v>51432</v>
       </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2251,7 +2293,7 @@
         <v>60000</v>
       </c>
       <c r="H10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2277,7 +2319,7 @@
         <v>66000</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2288,13 +2330,13 @@
         <v>44</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D12">
         <v>364</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" t="s">
         <v>9</v>
@@ -2303,7 +2345,7 @@
         <v>66000</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -2311,25 +2353,51 @@
         <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" t="s">
-        <v>46</v>
+        <v>55</v>
+      </c>
+      <c r="D13">
+        <v>455</v>
       </c>
       <c r="E13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>46</v>
+        <v>12</v>
       </c>
       <c r="G13" s="5">
         <v>70200</v>
       </c>
       <c r="H13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>56</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F14" t="s">
+        <v>60</v>
+      </c>
+      <c r="G14" s="5">
+        <v>90000</v>
+      </c>
+      <c r="H14" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update salary page, minor readme updates for my own benefit
</commit_message>
<xml_diff>
--- a/salary-transparency.xlsx
+++ b/salary-transparency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcali\Desktop\Repositories\pingzing.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC6F034-8E78-41F2-B58F-C7A76FBE0DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578AB6F-547D-4C20-9330-83F64DD975CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3DD130F-2BA7-4CF7-A266-8FC2D1A3BE0F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3DD130F-2BA7-4CF7-A266-8FC2D1A3BE0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
   <si>
     <t>Title</t>
   </si>
@@ -36,9 +36,6 @@
     <t>End</t>
   </si>
   <si>
-    <t>Days Worked</t>
-  </si>
-  <si>
     <t>Salary</t>
   </si>
   <si>
@@ -208,6 +205,18 @@
   </si>
   <si>
     <t>Terminated</t>
+  </si>
+  <si>
+    <t>Lead Software Engineer</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>€6350 EUR / month</t>
+  </si>
+  <si>
+    <t>Total Days</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Annual Salary &amp; Days Worked</a:t>
+              <a:t> Annual Salary &amp; Total Days at That Level</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -433,9 +442,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$14</c:f>
+              <c:f>Sheet1!$B$2:$B$15</c:f>
               <c:strCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>2013-06-01</c:v>
                 </c:pt>
@@ -474,16 +483,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2023-08-01</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2023-11-06</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$14</c:f>
+              <c:f>Sheet1!$G$2:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
                 </c:pt>
@@ -522,6 +534,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>76200</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -551,7 +566,15 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Days Worked</c:v>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total Days</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -570,9 +593,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$2:$C$14</c:f>
+              <c:f>Sheet1!$B$2:$C$15</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>2014-06-01</c:v>
@@ -653,6 +676,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>2023-08-01</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2023-11-06</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -660,10 +686,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$14</c:f>
+              <c:f>Sheet1!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>365</c:v>
                 </c:pt>
@@ -806,7 +832,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2940000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2940000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -2019,10 +2045,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDAF2D-9C38-457B-A68E-C11A0F37BCCC}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2047,357 +2073,374 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" t="s">
         <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="D2">
         <v>365</v>
       </c>
       <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
       </c>
       <c r="G2" s="5">
         <v>48000</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>298</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
         <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
       </c>
       <c r="G3" s="5">
         <v>57600</v>
       </c>
       <c r="H3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>506</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="5">
         <v>30252</v>
       </c>
       <c r="H4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>123</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G5" s="5">
         <v>32767</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6">
         <v>180</v>
       </c>
       <c r="E6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G6" s="5">
         <v>38640</v>
       </c>
       <c r="H6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="D7">
         <v>214</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G7" s="5">
         <v>42684</v>
       </c>
       <c r="H7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8">
         <v>423</v>
       </c>
       <c r="E8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G8" s="5">
         <v>47312</v>
       </c>
       <c r="H8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9">
         <v>291</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G9" s="5">
         <v>51432</v>
       </c>
       <c r="H9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="D10">
         <v>186</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G10" s="5">
         <v>60000</v>
       </c>
       <c r="H10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="D11">
         <v>272</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G11" s="5">
         <v>66000</v>
       </c>
       <c r="H11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12">
         <v>364</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G12" s="5">
         <v>66000</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13">
         <v>455</v>
       </c>
       <c r="E13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G13" s="5">
         <v>70200</v>
       </c>
       <c r="H13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="D14">
         <v>30</v>
       </c>
       <c r="E14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" t="s">
         <v>59</v>
-      </c>
-      <c r="F14" t="s">
-        <v>60</v>
       </c>
       <c r="G14" s="5">
         <v>90000</v>
       </c>
       <c r="H14" t="s">
-        <v>54</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="5">
+        <v>76200</v>
+      </c>
+      <c r="H15" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update salary transparency page
</commit_message>
<xml_diff>
--- a/salary-transparency.xlsx
+++ b/salary-transparency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcali\Desktop\Repositories\pingzing.github.io\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9578AB6F-547D-4C20-9330-83F64DD975CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74D18FCA-9ED7-432C-9317-050725C9B25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3DD130F-2BA7-4CF7-A266-8FC2D1A3BE0F}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D3DD130F-2BA7-4CF7-A266-8FC2D1A3BE0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
   <si>
     <t>Title</t>
   </si>
@@ -217,6 +217,18 @@
   </si>
   <si>
     <t>Total Days</t>
+  </si>
+  <si>
+    <t>2024-04-30</t>
+  </si>
+  <si>
+    <t>2024-05-01</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>€3000 EUR / month + 50% billed</t>
   </si>
 </sst>
 </file>
@@ -442,9 +454,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$2:$B$15</c:f>
+              <c:f>Sheet1!$B$2:$B$16</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2013-06-01</c:v>
                 </c:pt>
@@ -486,16 +498,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2023-11-06</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2024-05-01</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$15</c:f>
+              <c:f>Sheet1!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
                 </c:pt>
@@ -537,6 +552,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>76200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -593,9 +611,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$B$2:$C$15</c:f>
+              <c:f>Sheet1!$B$2:$C$16</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>2014-06-01</c:v>
@@ -635,6 +653,12 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>2023-08-31</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>2024-04-30</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>N/A</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -679,6 +703,9 @@
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>2023-11-06</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>2024-05-01</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -728,6 +755,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>176</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,8 +1747,8 @@
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1581149</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2045,10 +2075,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52DDAF2D-9C38-457B-A68E-C11A0F37BCCC}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2433,13 +2463,48 @@
       <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>176</v>
+      </c>
       <c r="E15" t="s">
         <v>62</v>
       </c>
+      <c r="F15" t="s">
+        <v>11</v>
+      </c>
       <c r="G15" s="5">
         <v>76200</v>
       </c>
       <c r="H15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>66</v>
+      </c>
+      <c r="E16" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" t="s">
+        <v>66</v>
+      </c>
+      <c r="G16" s="5">
+        <v>100800</v>
+      </c>
+      <c r="H16" t="s">
         <v>53</v>
       </c>
     </row>

</xml_diff>